<commit_message>
done ! this works theres one type in 04/15/2009 that needs to be fixed mannually.
</commit_message>
<xml_diff>
--- a/Files/Vaccine_April 1, 2013.xlsx
+++ b/Files/Vaccine_April 1, 2013.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="339">
   <si>
     <t xml:space="preserve">Vaccine</t>
   </si>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">Contract Number</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP [1]</t>
+    <t xml:space="preserve">DTaP </t>
   </si>
   <si>
     <t xml:space="preserve">Daptacel</t>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">$21.44</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP-IPV [2]</t>
+    <t xml:space="preserve">DTaP-IPV </t>
   </si>
   <si>
     <t xml:space="preserve">Kinrix</t>
@@ -116,7 +116,7 @@
     <t xml:space="preserve">10 pack - 1 dose T-L syringes</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP-Hep B-IPV [4]</t>
+    <t xml:space="preserve">DTaP-Hep B-IPV </t>
   </si>
   <si>
     <t xml:space="preserve">Pediarix</t>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">$70.72</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP-IP-HI [4]</t>
+    <t xml:space="preserve">DTaP-IP-HI </t>
   </si>
   <si>
     <t xml:space="preserve">Pentacel</t>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">$80.43</t>
   </si>
   <si>
-    <t xml:space="preserve">e-IPV [5]</t>
+    <t xml:space="preserve">e-IPV </t>
   </si>
   <si>
     <t xml:space="preserve">IPOL</t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">$27.44</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis B-Hib [3]</t>
+    <t xml:space="preserve">Hepatitis B-Hib </t>
   </si>
   <si>
     <t xml:space="preserve">Comvax</t>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">200-2013-54509</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis A Pediatric [5]</t>
+    <t xml:space="preserve">Hepatitis A Pediatric </t>
   </si>
   <si>
     <t xml:space="preserve">Vaqta</t>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">58160-0825-52</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis A-Hepatitis B 18 only [3]</t>
+    <t xml:space="preserve">Hepatitis A-Hepatitis B 18 only </t>
   </si>
   <si>
     <t xml:space="preserve">Twinrix</t>
@@ -254,8 +254,7 @@
     <t xml:space="preserve">58160-0815-52</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis B [5]
-Pediatric/Adolescent</t>
+    <t xml:space="preserve">Hepatitis B  Pediatric/Adolescent</t>
   </si>
   <si>
     <t xml:space="preserve">Engerix B</t>
@@ -273,8 +272,7 @@
     <t xml:space="preserve">58160-0820-52</t>
   </si>
   <si>
-    <t xml:space="preserve">Recombivax
-HB</t>
+    <t xml:space="preserve">Recombivax HB</t>
   </si>
   <si>
     <t xml:space="preserve">00006-4981-00</t>
@@ -295,7 +293,7 @@
     <t xml:space="preserve">$23.95</t>
   </si>
   <si>
-    <t xml:space="preserve">Hib [5]</t>
+    <t xml:space="preserve">Hib </t>
   </si>
   <si>
     <t xml:space="preserve">PedvaxHIB</t>
@@ -322,7 +320,7 @@
     <t xml:space="preserve">$26.21</t>
   </si>
   <si>
-    <t xml:space="preserve">HPV - Quadrivalent Human Papillomavirus Types 6, 11, 16 and 18 Recombinant [5]</t>
+    <t xml:space="preserve">HPV - Quadrivalent Human Papillomavirus Types 6, 11, 16 and 18 Recombinant </t>
   </si>
   <si>
     <t xml:space="preserve">Gardasil</t>
@@ -337,7 +335,7 @@
     <t xml:space="preserve">$135.453</t>
   </si>
   <si>
-    <t xml:space="preserve">HPV -Bivalent Human Papillomavirus Types 16 and 18 [5]</t>
+    <t xml:space="preserve">HPV -Bivalent Human Papillomavirus Types 16 and 18 </t>
   </si>
   <si>
     <t xml:space="preserve">Cervarix</t>
@@ -355,7 +353,7 @@
     <t xml:space="preserve">$128.75</t>
   </si>
   <si>
-    <t xml:space="preserve">Meningococcal Conjugate (Groups A, C, Y and W-135) [5]</t>
+    <t xml:space="preserve">Meningococcal Conjugate (Groups A, C, Y and W-135) </t>
   </si>
   <si>
     <t xml:space="preserve">Menactra</t>
@@ -391,7 +389,7 @@
     <t xml:space="preserve">200-2013-54511</t>
   </si>
   <si>
-    <t xml:space="preserve">Measles, Mumps and Rubella (MMR) [1]</t>
+    <t xml:space="preserve">Measles, Mumps and Rubella (MMR) </t>
   </si>
   <si>
     <t xml:space="preserve">M-M-RII</t>
@@ -406,7 +404,7 @@
     <t xml:space="preserve">$54.066</t>
   </si>
   <si>
-    <t xml:space="preserve">MMR/Varicella [2]</t>
+    <t xml:space="preserve">MMR/Varicella </t>
   </si>
   <si>
     <t xml:space="preserve">ProQuad</t>
@@ -421,8 +419,7 @@
     <t xml:space="preserve">$144.615</t>
   </si>
   <si>
-    <t xml:space="preserve">Pneumococcal
-13-valent [5] (Pediatric)</t>
+    <t xml:space="preserve">Pneumococcal 13-valent  (Pediatric)</t>
   </si>
   <si>
     <t xml:space="preserve">Prevnar 13 TM</t>
@@ -461,7 +458,7 @@
     <t xml:space="preserve">$64.422</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotavirus, Live, Oral, Pentavalent [5]</t>
+    <t xml:space="preserve">Rotavirus, Live, Oral, Pentavalent </t>
   </si>
   <si>
     <t xml:space="preserve">RotaTeq</t>
@@ -485,7 +482,7 @@
     <t xml:space="preserve">25 pack - 1 dose 2mL tubes</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotavirus, Live, Oral, Oral [5]</t>
+    <t xml:space="preserve">Rotavirus, Live, Oral, Oral </t>
   </si>
   <si>
     <t xml:space="preserve">Rotarix</t>
@@ -500,7 +497,7 @@
     <t xml:space="preserve">$106.57</t>
   </si>
   <si>
-    <t xml:space="preserve">Tetanus  Diphtheria Toxoids [3]</t>
+    <t xml:space="preserve">Tetanus  Diphtheria Toxoids </t>
   </si>
   <si>
     <t xml:space="preserve">Tenivac Effective Feb 1, 2013</t>
@@ -509,8 +506,7 @@
     <t xml:space="preserve">49281-0215-15</t>
   </si>
   <si>
-    <t xml:space="preserve">10 pack - 1 dose syringes
-No Needle</t>
+    <t xml:space="preserve">10 pack - 1 dose syringes No Needle</t>
   </si>
   <si>
     <t xml:space="preserve">$17.57</t>
@@ -522,7 +518,7 @@
     <t xml:space="preserve">49281-0215-10</t>
   </si>
   <si>
-    <t xml:space="preserve">Tetanus Toxoid, Reduced Diphtheria Toxoid and Acellular Pertussis [1]</t>
+    <t xml:space="preserve">Tetanus Toxoid, Reduced Diphtheria Toxoid and Acellular Pertussis </t>
   </si>
   <si>
     <t xml:space="preserve">Boostrix</t>
@@ -555,7 +551,7 @@
     <t xml:space="preserve">5 pack - 1 dose BD Leur-Lok syringes</t>
   </si>
   <si>
-    <t xml:space="preserve">Varicella [5]</t>
+    <t xml:space="preserve">Varicella </t>
   </si>
   <si>
     <t xml:space="preserve">Varivax</t>
@@ -570,7 +566,7 @@
     <t xml:space="preserve">$90.549</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis A Adult [5]</t>
+    <t xml:space="preserve">Hepatitis A Adult </t>
   </si>
   <si>
     <t xml:space="preserve">58160-0826-11</t>
@@ -591,7 +587,7 @@
     <t xml:space="preserve">$63.10</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis A-Adult [5]</t>
+    <t xml:space="preserve">Hepatitis A-Adult </t>
   </si>
   <si>
     <t xml:space="preserve">00006-4096-09</t>
@@ -609,13 +605,13 @@
     <t xml:space="preserve">200-2012-51349</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis A-Hepatitis B Adult [3]</t>
+    <t xml:space="preserve">Hepatitis A-Hepatitis B Adult </t>
   </si>
   <si>
     <t xml:space="preserve">$45.11</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis B-Adult [5]</t>
+    <t xml:space="preserve">Hepatitis B-Adult </t>
   </si>
   <si>
     <t xml:space="preserve">ENGERIX-B</t>
@@ -636,9 +632,6 @@
     <t xml:space="preserve">$26.19</t>
   </si>
   <si>
-    <t xml:space="preserve">Recombivax HB</t>
-  </si>
-  <si>
     <t xml:space="preserve">00006-4995-41</t>
   </si>
   <si>
@@ -669,13 +662,13 @@
     <t xml:space="preserve">$61.22</t>
   </si>
   <si>
-    <t xml:space="preserve">HPV -Quadrivalent Human Papillomavirus Types 6, 11, 16 and 18 Recombinant Adult [5]</t>
+    <t xml:space="preserve">HPV -Quadrivalent Human Papillomavirus Types 6, 11, 16 and 18 Recombinant Adult </t>
   </si>
   <si>
     <t xml:space="preserve">$90.402</t>
   </si>
   <si>
-    <t xml:space="preserve">HPV-Human Papillomavirus Bivalent Types 16 and 18 [5]</t>
+    <t xml:space="preserve">HPV-Human Papillomavirus Bivalent Types 16 and 18 </t>
   </si>
   <si>
     <t xml:space="preserve">10 pack - 1 dose T-L syringe, No Needle</t>
@@ -684,7 +677,7 @@
     <t xml:space="preserve">$77.60</t>
   </si>
   <si>
-    <t xml:space="preserve">Measles, Mumps,  Rubella-Adult [1]</t>
+    <t xml:space="preserve">Measles, Mumps,  Rubella-Adult </t>
   </si>
   <si>
     <t xml:space="preserve">$37.171</t>
@@ -732,7 +725,7 @@
     <t xml:space="preserve">$24.012</t>
   </si>
   <si>
-    <t xml:space="preserve">Varicella-Adult [5]</t>
+    <t xml:space="preserve">Varicella-Adult </t>
   </si>
   <si>
     <t xml:space="preserve">$60.883</t>
@@ -759,9 +752,6 @@
     <t xml:space="preserve">00006-4133-41</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
     <t xml:space="preserve">$13.108</t>
   </si>
   <si>
@@ -780,7 +770,7 @@
     <t xml:space="preserve">$13.317</t>
   </si>
   <si>
-    <t xml:space="preserve">Meningococcal Conjugate [5]</t>
+    <t xml:space="preserve">Meningococcal Conjugate </t>
   </si>
   <si>
     <t xml:space="preserve">$68.022</t>
@@ -792,8 +782,7 @@
     <t xml:space="preserve">$72.494</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5, 6]
-(Age 6 months and older)</t>
+    <t xml:space="preserve">Influenza  (Age 6 months and older)</t>
   </si>
   <si>
     <t xml:space="preserve">Fluzone</t>
@@ -811,13 +800,10 @@
     <t xml:space="preserve">200-2013-54015</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5]
-(Age 6-35 months)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluzone
-Pediatric dose
-No Preservative</t>
+    <t xml:space="preserve">Influenza  (Age 6-35 months)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluzone Pediatric dose No Preservative</t>
   </si>
   <si>
     <t xml:space="preserve">49281-0113-25</t>
@@ -826,12 +812,10 @@
     <t xml:space="preserve">$12.227</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5]
-(Age 36 months and older)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluzone
-No-Preservative</t>
+    <t xml:space="preserve">Influenza  (Age 36 months and older)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluzone No-Preservative</t>
   </si>
   <si>
     <t xml:space="preserve">49281-0013-50</t>
@@ -852,15 +836,13 @@
     <t xml:space="preserve">$13.075</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluarix
-Preservative Free</t>
+    <t xml:space="preserve">Fluarix Preservative Free</t>
   </si>
   <si>
     <t xml:space="preserve">58160-0880-52</t>
   </si>
   <si>
-    <t xml:space="preserve">10 pack- 1 dose
-TipLok syringe</t>
+    <t xml:space="preserve">10 pack- 1 dose TipLok syringe</t>
   </si>
   <si>
     <t xml:space="preserve">$9.25</t>
@@ -872,8 +854,7 @@
     <t xml:space="preserve">200-2013-54020</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluarix Quadrivalent
-Preservative Free</t>
+    <t xml:space="preserve">Fluarix Quadrivalent Preservative Free</t>
   </si>
   <si>
     <t xml:space="preserve">58160-0900-52</t>
@@ -885,8 +866,7 @@
     <t xml:space="preserve">15.90</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5, 6]
-(Age 4 years and older)</t>
+    <t xml:space="preserve">Influenza  (Age 4 years and older)</t>
   </si>
   <si>
     <t xml:space="preserve">Fluvirin</t>
@@ -904,8 +884,7 @@
     <t xml:space="preserve">200-2013-54019</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluvirin
-Preservative Free</t>
+    <t xml:space="preserve">Fluvirin Preservative Free</t>
   </si>
   <si>
     <t xml:space="preserve">66521-0116-02</t>
@@ -920,12 +899,10 @@
     <t xml:space="preserve">$14.35</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5]
-Live, Intranasal (Age 2-49 years)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FluMist
-No Preservative Quadrivalent</t>
+    <t xml:space="preserve">Influenza  Live, Intranasal (Age 2-49 years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FluMist No Preservative Quadrivalent</t>
   </si>
   <si>
     <t xml:space="preserve">TBA</t>
@@ -946,32 +923,24 @@
     <t xml:space="preserve">200-2013-54017</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5]
-(Age 9 years and older)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afluria
-No Preservative</t>
+    <t xml:space="preserve">Influenza  (Age 9 years and older)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afluria No Preservative</t>
   </si>
   <si>
     <t xml:space="preserve">33332-0013-01</t>
   </si>
   <si>
-    <t xml:space="preserve">10 pack-1 dose
-syringe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merck
-(CSL product)</t>
+    <t xml:space="preserve">10 pack-1 dose syringe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merck (CSL product)</t>
   </si>
   <si>
     <t xml:space="preserve">200-2013-54016</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5, 6]
-(Age 9 years and older)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Afluria</t>
   </si>
   <si>
@@ -993,8 +962,7 @@
     <t xml:space="preserve">200-2013-54009</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5]
-(Age 18 - 64 years)</t>
+    <t xml:space="preserve">Influenza  (Age 18 - 64 years)</t>
   </si>
   <si>
     <t xml:space="preserve">49281-0707-55</t>
@@ -1006,8 +974,7 @@
     <t xml:space="preserve">$16.72</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluzone
-No Preservative</t>
+    <t xml:space="preserve">Fluzone No Preservative</t>
   </si>
   <si>
     <t xml:space="preserve">$9.494</t>
@@ -1016,8 +983,7 @@
     <t xml:space="preserve">$9.93</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5]
-(Age 18 years and older)</t>
+    <t xml:space="preserve">Influenza  (Age 18 years and older)</t>
   </si>
   <si>
     <t xml:space="preserve">Flucelvax Preservative Free Antibiotic free</t>
@@ -1038,15 +1004,7 @@
     <t xml:space="preserve">$6.75</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza [5]
-(Age 4 years and older)</t>
-  </si>
-  <si>
     <t xml:space="preserve">$7.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Influenza [5, 6]
-(Age 18 years and older)</t>
   </si>
   <si>
     <t xml:space="preserve">FluLaval</t>
@@ -2590,19 +2548,19 @@
         <v>198</v>
       </c>
       <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
         <v>205</v>
-      </c>
-      <c r="C9" t="s">
-        <v>206</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F9" t="s">
         <v>207</v>
-      </c>
-      <c r="F9" t="s">
-        <v>208</v>
       </c>
       <c r="G9" s="1">
         <v>41455</v>
@@ -2619,19 +2577,19 @@
         <v>198</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" t="s">
         <v>209</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>210</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>211</v>
-      </c>
-      <c r="F10" t="s">
-        <v>212</v>
       </c>
       <c r="G10" s="1">
         <v>41455</v>
@@ -2648,19 +2606,19 @@
         <v>198</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D11" t="s">
         <v>213</v>
-      </c>
-      <c r="D11" t="s">
-        <v>214</v>
       </c>
       <c r="E11" t="s">
         <v>204</v>
       </c>
       <c r="F11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G11" s="1">
         <v>41455</v>
@@ -2674,7 +2632,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" t="s">
         <v>102</v>
@@ -2686,7 +2644,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F12" t="s">
         <v>105</v>
@@ -2703,7 +2661,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" t="s">
         <v>107</v>
@@ -2712,10 +2670,10 @@
         <v>108</v>
       </c>
       <c r="D13" t="s">
+        <v>218</v>
+      </c>
+      <c r="E13" t="s">
         <v>219</v>
-      </c>
-      <c r="E13" t="s">
-        <v>220</v>
       </c>
       <c r="F13" t="s">
         <v>111</v>
@@ -2732,7 +2690,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B14" t="s">
         <v>125</v>
@@ -2744,7 +2702,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F14" t="s">
         <v>128</v>
@@ -2767,16 +2725,16 @@
         <v>143</v>
       </c>
       <c r="C15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D15" t="s">
         <v>223</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>224</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>225</v>
-      </c>
-      <c r="F15" t="s">
-        <v>226</v>
       </c>
       <c r="G15" s="1">
         <v>41455</v>
@@ -2799,10 +2757,10 @@
         <v>144</v>
       </c>
       <c r="D16" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" t="s">
         <v>227</v>
-      </c>
-      <c r="E16" t="s">
-        <v>228</v>
       </c>
       <c r="F16" t="s">
         <v>146</v>
@@ -2831,7 +2789,7 @@
         <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F17" t="s">
         <v>171</v>
@@ -2854,13 +2812,13 @@
         <v>168</v>
       </c>
       <c r="C18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D18" t="s">
         <v>230</v>
       </c>
-      <c r="D18" t="s">
-        <v>231</v>
-      </c>
       <c r="E18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F18" t="s">
         <v>171</v>
@@ -2889,7 +2847,7 @@
         <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F19" t="s">
         <v>175</v>
@@ -2898,10 +2856,10 @@
         <v>41455</v>
       </c>
       <c r="H19" t="s">
+        <v>232</v>
+      </c>
+      <c r="I19" t="s">
         <v>233</v>
-      </c>
-      <c r="I19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="20">
@@ -2915,10 +2873,10 @@
         <v>176</v>
       </c>
       <c r="D20" t="s">
+        <v>234</v>
+      </c>
+      <c r="E20" t="s">
         <v>235</v>
-      </c>
-      <c r="E20" t="s">
-        <v>236</v>
       </c>
       <c r="F20" t="s">
         <v>175</v>
@@ -2927,15 +2885,15 @@
         <v>41455</v>
       </c>
       <c r="H20" t="s">
+        <v>232</v>
+      </c>
+      <c r="I20" t="s">
         <v>233</v>
-      </c>
-      <c r="I20" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s">
         <v>179</v>
@@ -2947,7 +2905,7 @@
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F21" t="s">
         <v>182</v>
@@ -2964,22 +2922,22 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22" t="s">
         <v>239</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>240</v>
-      </c>
-      <c r="C22" t="s">
-        <v>241</v>
       </c>
       <c r="D22" t="s">
         <v>54</v>
       </c>
       <c r="E22" t="s">
+        <v>241</v>
+      </c>
+      <c r="F22" t="s">
         <v>242</v>
-      </c>
-      <c r="F22" t="s">
-        <v>243</v>
       </c>
       <c r="G22" s="1">
         <v>41455</v>
@@ -2993,22 +2951,19 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23" t="s">
         <v>244</v>
-      </c>
-      <c r="B23" t="s">
-        <v>245</v>
-      </c>
-      <c r="C23" t="s">
-        <v>246</v>
       </c>
       <c r="D23" t="s">
         <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F23" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G23" s="1">
         <v>41455</v>
@@ -3022,10 +2977,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C24" t="s">
         <v>166</v>
@@ -3034,7 +2989,7 @@
         <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F24" t="s">
         <v>165</v>
@@ -3043,27 +2998,27 @@
         <v>41455</v>
       </c>
       <c r="H24" t="s">
+        <v>232</v>
+      </c>
+      <c r="I24" t="s">
         <v>233</v>
-      </c>
-      <c r="I24" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B25" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C25" t="s">
         <v>162</v>
       </c>
       <c r="D25" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E25" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F25" t="s">
         <v>165</v>
@@ -3072,15 +3027,15 @@
         <v>41455</v>
       </c>
       <c r="H25" t="s">
+        <v>232</v>
+      </c>
+      <c r="I25" t="s">
         <v>233</v>
-      </c>
-      <c r="I25" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B26" t="s">
         <v>118</v>
@@ -3092,7 +3047,7 @@
         <v>115</v>
       </c>
       <c r="E26" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F26" t="s">
         <v>121</v>
@@ -3104,12 +3059,12 @@
         <v>122</v>
       </c>
       <c r="I26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B27" t="s">
         <v>113</v>
@@ -3121,7 +3076,7 @@
         <v>115</v>
       </c>
       <c r="E27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F27" t="s">
         <v>117</v>
@@ -3130,10 +3085,10 @@
         <v>41455</v>
       </c>
       <c r="H27" t="s">
+        <v>232</v>
+      </c>
+      <c r="I27" t="s">
         <v>233</v>
-      </c>
-      <c r="I27" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3183,22 +3138,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" t="s">
         <v>257</v>
-      </c>
-      <c r="B2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" t="s">
-        <v>259</v>
       </c>
       <c r="D2" t="s">
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G2" s="1">
         <v>41691</v>
@@ -3207,24 +3162,24 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" t="s">
         <v>263</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" t="s">
         <v>264</v>
-      </c>
-      <c r="C3" t="s">
-        <v>265</v>
-      </c>
-      <c r="D3" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" t="s">
-        <v>266</v>
       </c>
       <c r="F3" t="s">
         <v>62</v>
@@ -3236,27 +3191,27 @@
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" t="s">
         <v>267</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" t="s">
         <v>268</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>269</v>
-      </c>
-      <c r="D4" t="s">
-        <v>251</v>
-      </c>
-      <c r="E4" t="s">
-        <v>270</v>
-      </c>
-      <c r="F4" t="s">
-        <v>271</v>
       </c>
       <c r="G4" s="1">
         <v>41691</v>
@@ -3265,27 +3220,27 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G5" s="1">
         <v>41691</v>
@@ -3294,27 +3249,27 @@
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" t="s">
         <v>275</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>276</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>277</v>
-      </c>
-      <c r="E6" t="s">
-        <v>278</v>
-      </c>
-      <c r="F6" t="s">
-        <v>279</v>
       </c>
       <c r="G6" s="1">
         <v>41691</v>
@@ -3323,27 +3278,27 @@
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E7" t="s">
         <v>281</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>282</v>
-      </c>
-      <c r="D7" t="s">
-        <v>277</v>
-      </c>
-      <c r="E7" t="s">
-        <v>283</v>
-      </c>
-      <c r="F7" t="s">
-        <v>284</v>
       </c>
       <c r="G7" s="1">
         <v>41691</v>
@@ -3352,27 +3307,27 @@
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" t="s">
         <v>285</v>
-      </c>
-      <c r="B8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C8" t="s">
-        <v>287</v>
       </c>
       <c r="D8" t="s">
         <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G8" s="1">
         <v>41691</v>
@@ -3381,27 +3336,27 @@
         <v>122</v>
       </c>
       <c r="I8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" t="s">
         <v>291</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>292</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>293</v>
-      </c>
-      <c r="E9" t="s">
-        <v>294</v>
-      </c>
-      <c r="F9" t="s">
-        <v>295</v>
       </c>
       <c r="G9" s="1">
         <v>41691</v>
@@ -3410,53 +3365,53 @@
         <v>122</v>
       </c>
       <c r="I9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10" t="s">
         <v>296</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>297</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>298</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>299</v>
-      </c>
-      <c r="E10" t="s">
-        <v>300</v>
-      </c>
-      <c r="F10" t="s">
-        <v>301</v>
       </c>
       <c r="G10" s="1">
         <v>41691</v>
       </c>
       <c r="H10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>302</v>
+      </c>
+      <c r="B11" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" t="s">
         <v>304</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>305</v>
       </c>
-      <c r="C11" t="s">
-        <v>306</v>
-      </c>
-      <c r="D11" t="s">
-        <v>307</v>
-      </c>
       <c r="E11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F11" t="s">
         <v>87</v>
@@ -3465,39 +3420,39 @@
         <v>41691</v>
       </c>
       <c r="H11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" t="s">
         <v>310</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>311</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>312</v>
-      </c>
-      <c r="D12" t="s">
-        <v>313</v>
-      </c>
-      <c r="E12" t="s">
-        <v>314</v>
-      </c>
-      <c r="F12" t="s">
-        <v>315</v>
       </c>
       <c r="G12" s="1">
         <v>41691</v>
       </c>
       <c r="H12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3547,22 +3502,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" t="s">
         <v>257</v>
-      </c>
-      <c r="B2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" t="s">
-        <v>259</v>
       </c>
       <c r="D2" t="s">
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G2" s="1">
         <v>41691</v>
@@ -3571,27 +3526,27 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" t="s">
+        <v>317</v>
+      </c>
+      <c r="F3" t="s">
         <v>318</v>
-      </c>
-      <c r="B3" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" t="s">
-        <v>319</v>
-      </c>
-      <c r="D3" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" t="s">
-        <v>320</v>
-      </c>
-      <c r="F3" t="s">
-        <v>321</v>
       </c>
       <c r="G3" s="1">
         <v>41691</v>
@@ -3600,27 +3555,27 @@
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C4" t="s">
         <v>267</v>
       </c>
-      <c r="B4" t="s">
-        <v>322</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F4" t="s">
         <v>269</v>
-      </c>
-      <c r="D4" t="s">
-        <v>251</v>
-      </c>
-      <c r="E4" t="s">
-        <v>323</v>
-      </c>
-      <c r="F4" t="s">
-        <v>271</v>
       </c>
       <c r="G4" s="1">
         <v>41691</v>
@@ -3629,27 +3584,27 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G5" s="1">
         <v>41691</v>
@@ -3658,27 +3613,27 @@
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D6" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" t="s">
         <v>325</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>326</v>
-      </c>
-      <c r="C6" t="s">
-        <v>327</v>
-      </c>
-      <c r="D6" t="s">
-        <v>251</v>
-      </c>
-      <c r="E6" t="s">
-        <v>328</v>
-      </c>
-      <c r="F6" t="s">
-        <v>329</v>
       </c>
       <c r="G6" s="1">
         <v>41691</v>
@@ -3687,27 +3642,27 @@
         <v>122</v>
       </c>
       <c r="I6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" t="s">
         <v>285</v>
-      </c>
-      <c r="B7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" t="s">
-        <v>287</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G7" s="1">
         <v>41691</v>
@@ -3716,27 +3671,27 @@
         <v>122</v>
       </c>
       <c r="I7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>332</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" t="s">
         <v>291</v>
       </c>
-      <c r="C8" t="s">
-        <v>292</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>329</v>
+      </c>
+      <c r="F8" t="s">
         <v>293</v>
-      </c>
-      <c r="E8" t="s">
-        <v>333</v>
-      </c>
-      <c r="F8" t="s">
-        <v>295</v>
       </c>
       <c r="G8" s="1">
         <v>41691</v>
@@ -3745,27 +3700,27 @@
         <v>122</v>
       </c>
       <c r="I8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="B9" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C9" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F9" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G9" s="1">
         <v>41691</v>
@@ -3774,27 +3729,27 @@
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E10" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G10" s="1">
         <v>41691</v>
@@ -3803,27 +3758,27 @@
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C11" t="s">
+        <v>280</v>
+      </c>
+      <c r="D11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" t="s">
+        <v>335</v>
+      </c>
+      <c r="F11" t="s">
         <v>282</v>
-      </c>
-      <c r="D11" t="s">
-        <v>251</v>
-      </c>
-      <c r="E11" t="s">
-        <v>340</v>
-      </c>
-      <c r="F11" t="s">
-        <v>284</v>
       </c>
       <c r="G11" s="1">
         <v>41691</v>
@@ -3832,24 +3787,24 @@
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" t="s">
         <v>304</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>305</v>
       </c>
-      <c r="C12" t="s">
-        <v>306</v>
-      </c>
-      <c r="D12" t="s">
-        <v>307</v>
-      </c>
       <c r="E12" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F12" t="s">
         <v>87</v>
@@ -3858,39 +3813,39 @@
         <v>41691</v>
       </c>
       <c r="H12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I12" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" t="s">
         <v>310</v>
       </c>
-      <c r="B13" t="s">
-        <v>311</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F13" t="s">
         <v>312</v>
-      </c>
-      <c r="D13" t="s">
-        <v>313</v>
-      </c>
-      <c r="E13" t="s">
-        <v>343</v>
-      </c>
-      <c r="F13" t="s">
-        <v>315</v>
       </c>
       <c r="G13" s="1">
         <v>41691</v>
       </c>
       <c r="H13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I13" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>